<commit_message>
Issue#22 Handle empty cells in ExcelSource
</commit_message>
<xml_diff>
--- a/ETLBoxTest/src/DataFlow/ExcelDataFile.xlsx
+++ b/ETLBoxTest/src/DataFlow/ExcelDataFile.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mac\Home\Github\roadrunnerlenny\etlbox\ETLBoxTest\src\DataFlow\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\mac\Home\Github\roadrunnerlenny\etlbox\ETLBoxTest\src\DataFlow\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56BB4C85-3512-4059-B703-C453A37F1BEF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F08E48E2-2F0F-43B0-A414-A63F3924EF3D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1725" windowWidth="18885" windowHeight="6668" activeTab="1" xr2:uid="{1377D143-6026-4458-9B5C-7B8A1C084738}"/>
+    <workbookView xWindow="2940" yWindow="3285" windowWidth="18900" windowHeight="10305" activeTab="1" xr2:uid="{1377D143-6026-4458-9B5C-7B8A1C084738}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="7">
   <si>
     <t>Col1</t>
   </si>
@@ -45,31 +45,10 @@
     <t>Wert1</t>
   </si>
   <si>
-    <t>Wert2</t>
-  </si>
-  <si>
-    <t>Wert3</t>
-  </si>
-  <si>
     <t>Wert4</t>
   </si>
   <si>
     <t>Wert5</t>
-  </si>
-  <si>
-    <t>1,0</t>
-  </si>
-  <si>
-    <t>1,1</t>
-  </si>
-  <si>
-    <t>1,2</t>
-  </si>
-  <si>
-    <t>1,3</t>
-  </si>
-  <si>
-    <t>1,4</t>
   </si>
   <si>
     <t>Invalid Values</t>
@@ -434,142 +413,142 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="B1" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="C1" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="D1" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="D3" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="D4" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="D5" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="D6" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="D8" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="C9" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="D9" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="B10" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="C10" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="D10" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -605,30 +584,24 @@
       <c r="C4" t="s">
         <v>3</v>
       </c>
-      <c r="D4" t="s">
-        <v>8</v>
+      <c r="D4">
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B5">
         <v>2</v>
       </c>
-      <c r="C5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" t="s">
-        <v>9</v>
+      <c r="D5">
+        <v>1.1000000000000001</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B6">
         <v>3</v>
       </c>
-      <c r="C6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" t="s">
-        <v>10</v>
+      <c r="D6">
+        <v>1.2</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.45">
@@ -636,10 +609,7 @@
         <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.45">
@@ -647,10 +617,10 @@
         <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" t="s">
-        <v>12</v>
+        <v>5</v>
+      </c>
+      <c r="D8">
+        <v>1.4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>